<commit_message>
feat: melhorias de UX
</commit_message>
<xml_diff>
--- a/data/Info RAG MD.xlsx
+++ b/data/Info RAG MD.xlsx
@@ -761,7 +761,7 @@
     <t>https://www.posuscs.com.br/melhores-alimentos-para-ajudar-na-cicatrizacao-no-pos-operatorio/noticia/3099</t>
   </si>
   <si>
-    <t>{"indicacoes": "[cicatrização, inflamação]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[cicatrização, inflamação]", "alimentos": "[Frango, Peru, carne bovina, Peixes, salmão, sardinha, Ovos, Leite, iogurte, queijo, Feijões, lentilhas, grão-de-bico, Laranjas, limões, toranjas, Morangos, kiwis, abacaxi, Pimentões, brócolis, espinafre, Cenouras, abóbora, batata-doce]"}</t>
   </si>
   <si>
     <t xml:space="preserve">ALIMENTOS PARA AJUDAR EM DISTÚRBIOS DIGESTIVOS
@@ -790,7 +790,7 @@
 https://www.clinicacirurgicataguatinga.com.br/voce-sabia-que-a-ma-alimentacao-pode-agravar-as-doencas-gastrointestinais/</t>
   </si>
   <si>
-    <t>{"indicacoes": "[digestão]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[digestão, distúrbios digestivos]", "alimentos": "[mamão, abacaxi, Água, chás, Azeite, castanhas, amêndoas, Cereais integrais, farinha de arroz, Vegetais]"}</t>
   </si>
   <si>
     <t>ALIMENTOS PARA AJUDAR A FADIGA
@@ -825,7 +825,7 @@
     <t>https://www.tuasaude.com/alimentos-que-combatem-o-cansaco/</t>
   </si>
   <si>
-    <t>{"indicacoes": "[fadiga]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[fadiga]", "alimentos": "[Maracujá, Abacate, Banana,Cereja,Alface,Canela,Chá de erva-cidreira,Mel,Amendoim,Ovos,Abóbora,Amêndoas,Espinafre,Aveia,Levedura de cerveja,Queijo,Cacau,Canela,Brócolis, Beterraba]"}</t>
   </si>
   <si>
     <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A DOR DE CABEÇA E ENXAQUECA
@@ -852,7 +852,7 @@
     <t>https://www.hcor.com.br/imprensa/noticias/alimentacao-balanceada-pode-ajudar-contra-as-crises-de-enxaqueca/</t>
   </si>
   <si>
-    <t>{"indicacoes": "[dor de sabeça, enxaqueca]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[dor de sabeça, enxaqueca]", "alimentos": "[Semente de linhaça, atum, sardinha, salmão, cavala, Castanhas, amêndoas, amendoim, banana, erva-cidreira, maracujá, pão, arroz, feijão, granola, orégano, cravo, canela, gengibre, amêndoas, avelã, castanha-do-pará, amendoim, alcachofra, espinafre, feijão, lentilha e grão de bico]"}</t>
   </si>
   <si>
     <t>ALIMENTOS PARA AJUDAR COM PROBLEMAS DE CIRCULAÇÃO
@@ -881,7 +881,7 @@
 No entanto, ela não substitui uma visita ao médico, principalmente se você estiver com sintomas que citamos acima e notar que algo não vai bem no seu corpo.</t>
   </si>
   <si>
-    <t>{"indicacoes": "[circulação]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[circulação]", "alimentos": "[Laranja, vitamina C, Gengibre, Alho, Cúrcuma, Salmão, atum, sardinha, Melão, melancia, Uva]"}</t>
   </si>
   <si>
     <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM PROBLEMAS DE CONCENTRAÇÃO E MEMÓRIA
@@ -902,7 +902,7 @@
     <t>https://www.sesipr.org.br/colegiosesi/internacional/alimentos-que-melhoram-sua-saude-e-auxiliam-na-concentracao-e-memoria-1-37143-431047.shtml</t>
   </si>
   <si>
-    <t>{"indicacoes": "[concentração, memória]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[concentração, memória]", "alimentos": "[frutas, barrinhas de cereais, torradas integrais, leite com aveia, peixes de água frita, soja, linhaça, frutos do mar, carnes, gema de ovo, carnes vermelhas, cereais integrais, alface, azeite de oliva, sálvia, água]"}</t>
   </si>
   <si>
     <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM PROBLEMAS RESPIRATÓRIOS
@@ -931,7 +931,7 @@
     <t>https://espacodevida.org.br/dicas-de-alimentacao-para-quem-esta-com-insuficiencia-respiratoria-de-qualquer-causa/</t>
   </si>
   <si>
-    <t>{"indicacoes": "[problemas respiratórios, asma]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[problemas respiratórios, asma]", "alimentos": "[alimentos pastosos, sucos, sopas, gengibre, alecrim, hortelã, limão, canela, guaco]"}</t>
   </si>
   <si>
     <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A GRIPE
@@ -947,7 +947,7 @@
     <t>https://www.hospitaloswaldocruz.org.br/imprensa/hospital-na-midia/bateu-a-gripe-veja-os-alimentos-que-ajudam-a-melhorar-a-imunidade-e-combater-a-doenca/</t>
   </si>
   <si>
-    <t>{"indicacoes": "[gripe]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[gripe]", "alimentos": "[vitamina C, laranja, limão, kiwi, acerola, tomate, peixes, ovos, carnes magras, legumes]"}</t>
   </si>
   <si>
     <t>ALIMENTOS PARA AJUDAR COM A FEBRE
@@ -991,7 +991,7 @@
     <t>https://www.cuf.pt/mais-saude/o-que-fazer-para-baixar-febre</t>
   </si>
   <si>
-    <t>{"indicacoes": "[febre]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[febre]", "alimentos": "[água, sumos, caldos]"}</t>
   </si>
   <si>
     <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM CONTUSÕES
@@ -1028,7 +1028,7 @@
     <t>https://encontrar.org.br/uma-boa-nutricao-pode-auxiliar-no-combate-aos-sintomas-da-artrose/</t>
   </si>
   <si>
-    <t>{"indicacoes": "[artrose]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[artrose]", "alimentos": "[frutas, ovo de galinha que cisca, leite,  queijo, peixe  sardinha, cavalinha, chia, Linhaça, vitamina D, cálcio, complexo B, Vitamina C, Vitamina E ,couve, cenoura, gengibre, maça, limão, água, alecrim, salsinha, cebolinha, manjericão, orégano, louro, páprica, pimenta do reino, alho e cebola, Banana, Laranja lima, Castanha do Pará , Mamão]"}</t>
   </si>
   <si>
     <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A ARTRITE
@@ -1075,7 +1075,7 @@
     <t>https://www.arthritis.org/health-wellness/healthy-living/nutrition/anti-inflammatory/the-ultimate-arthritis-diet</t>
   </si>
   <si>
-    <t>{"indicacoes": "[artrite]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[artrite]", "alimentos": "[peixes, nozes, sementes, frutas, vegetais, azeite, feijões]"}</t>
   </si>
   <si>
     <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM CISTITE
@@ -1115,7 +1115,7 @@
     <t>https://femalehealthawareness.org/en/nutritional-considerations-for-a-healthy-menstrual-cycle/</t>
   </si>
   <si>
-    <t>{"indicacoes": "[menstruação]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[menstruação irregular]", "alimentos": "[vegetais, proteínas, vitamina D, nozes, leguminosas, grãos integrais]"}</t>
   </si>
   <si>
     <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A CÓLICA
@@ -1147,7 +1147,7 @@
     <t>https://hospitalsiriolibanes.org.br/blog/ginecologia/dicas-colica-menstrual</t>
   </si>
   <si>
-    <t>{"indicacoes": "[cólica]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[cólica menstrual]", "alimentos": "[ bolsas térmicas, chá de Camomila, chá de Erva-doce, chá de Gengibre, meditação, tomar um banho morno, banana, espinafre, abacate e sementes, peixes, linhaça, chia, frutas, legumes, grãos integrais]"}</t>
   </si>
   <si>
     <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM TENSÃO PRÉ-MENSTRUAL
@@ -1175,7 +1175,7 @@
     <t>https://www.gov.br/saude/pt-br/assuntos/saude-brasil/eu-quero-me-alimentar-melhor/noticias/2018/cinco-alimentos-para-enfrentar-melhor-a-tpm</t>
   </si>
   <si>
-    <t>{"indicacoes": "[TPM]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[TPM]", "alimentos": "[feijão, lentilha, ervilhas, Banana, Aveia, Peixes de mar profundo, Verduras escuras]"}</t>
   </si>
   <si>
     <t>ALIMENTOS PARA AJUDAR COM QUEIMADURAS
@@ -1194,20 +1194,20 @@
     <t>https://msktc.org/burn/factsheets/healthy-eating-after-burn-injury-adults</t>
   </si>
   <si>
-    <t>{"indicacoes": "[queimadura]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[queimadura]", "alimentos": "[carnes magras, grãos integrais, vegetais, frutas, laticínios,carne bovina, frango, carne suína, ovos, feijão, nozes, leite, iogurte, queijo]"}</t>
   </si>
   <si>
     <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM DERMATITES
 INDICAÇÕES:
 Peixe: Os ácidos gordos ómega 3 encontrados no peixe, como no salmão, atum, sardinhas ou mesmo no marisco, possuem propriedades anti-inflamatórias que combatem os danos causados pela exposição prolongada ao sol. Legumes folhas verdes: A vitamina A combate o envelhecimento precoce, a formação de escamas e a desidratação. Também é essencial para a renovação celular e promove o crescimento de nova pele. “Os espinafres e brócolis, por exemplo, são excelentes fontes de vitamina A”. Citrinos: A vitamina C é um antioxidante muito poderoso que pode manter o colágeno na estrutura da pele e impedir a flacidez. “Laranjas, mexericas, limões e limas são também excelentes escolhas”.
 Água:  a água estimula o trânsito intestinal e a eliminação de toxinas do organismo, impedindo que o seu acúmulo seja refletido na pele. “A ingestão recomendada é de oito copos ou 2 litros/dia. Se não houver boa hidratação, podem ocorrer constipação intestinal, aumento de celulite, problemas renais, pele e cabelos ressecados e desidratados. Para aumentar a hidratação, é necessário obrigar-se a beber água. Um bom parâmetro para verificar maior necessidade de líquido é a cor da urina (quanto mais escura, maior a necessidade de água)”.
-CUIDADOS: </t>
+</t>
   </si>
   <si>
     <t>https://cdd.org.br/noticias/saiba-como-a-alimentacao-influencia-nas-dermatites/</t>
   </si>
   <si>
-    <t>{"indicacoes": "[dermatite]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[dermatite]", "alimentos": "[peixes, água]"}</t>
   </si>
   <si>
     <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM QUEDA DE CABELO
@@ -1228,7 +1228,7 @@
     <t>https://sbdrs.org.br/saiba-quais-alimentos-ajudam-a-garantir-a-saude-dos-cabelos/</t>
   </si>
   <si>
-    <t>{"indicacoes": "[queda de cabelo]", "alimentos": "[]"}</t>
+    <t>{"indicacoes": "[queda de cabelo]", "alimentos": "[proteínas, aminoácidos, minerais, biotina, além de certos tipos de óleos e antioxidantes, salmão, arenque, sardinha e atum, ovos, espinafre, couve e rúcula, frutas cítricas, nozes, castanha-do-pará]"}</t>
   </si>
   <si>
     <t xml:space="preserve">ALIMENTOS PARA AJUDAR COM A ACNE

</xml_diff>